<commit_message>
Logout; MD5 Hash für PW; abfangen wenn Nutzer bereits existiert
</commit_message>
<xml_diff>
--- a/todos.xlsx
+++ b/todos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>abfangen wenn kein Bild hochgeladen oder Datum angegeben</t>
   </si>
@@ -48,16 +48,32 @@
   </si>
   <si>
     <t xml:space="preserve">abfangen, wenn Datum bereits vorbei </t>
+  </si>
+  <si>
+    <t>Passwort verschlüsseln (wenigstens MD5 Hash)</t>
+  </si>
+  <si>
+    <t>erledigr</t>
+  </si>
+  <si>
+    <t>erledigt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -365,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,7 +393,7 @@
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,7 +401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -392,30 +409,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exception Handling, wenn nicht alle Daten angegeben wurden bei newProduct.php; Fehlt nur noch, wenn kein image hochgeladen wurde.
Update todos.xlsx
</commit_message>
<xml_diff>
--- a/todos.xlsx
+++ b/todos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>abfangen wenn kein Bild hochgeladen oder Datum angegeben</t>
   </si>
@@ -57,13 +57,62 @@
   </si>
   <si>
     <t>erledigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produkte werden iwie komisch aufgelistet, wenn zu viele </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nur wenn man kein bild hochgeladen hat kommt noch ne Fehlermeldung </t>
+  </si>
+  <si>
+    <r>
+      <t>warning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: file_get_contents(): Filename cannot be empty in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>D:\Programme und Funktionen\Xampp\xampp\htdocs\EbayFuerArme\newProduct.php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> on line </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>144</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +123,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,9 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -117,6 +188,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3631083</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>187722</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3631083" y="1819275"/>
+          <a:ext cx="3198342" cy="1606947"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -393,15 +507,28 @@
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -409,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -422,7 +549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -433,17 +560,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -454,8 +581,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>